<commit_message>
Integración ExcelSync: sincronización automática de trabajadores y exclusión del admin
</commit_message>
<xml_diff>
--- a/Backend/python/Carta_output.xlsx
+++ b/Backend/python/Carta_output.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>Trabajador</t>
   </si>
@@ -57,139 +57,127 @@
     <t>Jocelyn</t>
   </si>
   <si>
+    <t>08:30 - 18:30</t>
+  </si>
+  <si>
+    <t>08:00 - 18:00</t>
+  </si>
+  <si>
     <t>11:00 - 21:00</t>
   </si>
   <si>
-    <t>08:00 - 18:00</t>
-  </si>
-  <si>
-    <t>08:30 - 18:30</t>
-  </si>
-  <si>
     <t>Ignacio</t>
   </si>
   <si>
     <t>Ingrid</t>
   </si>
   <si>
+    <t>13:00 - 20:00</t>
+  </si>
+  <si>
+    <t>11:00 - 18:00</t>
+  </si>
+  <si>
     <t>12:00 - 19:00</t>
   </si>
   <si>
     <t>14:30 - 21:30</t>
   </si>
   <si>
+    <t>Agustin</t>
+  </si>
+  <si>
+    <t>16:30 - 23:30</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>17:30 - 23:30</t>
+  </si>
+  <si>
+    <t>13:00 - 21:00</t>
+  </si>
+  <si>
     <t>10:00 - 17:00</t>
   </si>
   <si>
+    <t>Franco</t>
+  </si>
+  <si>
+    <t>14:30 - 20:30</t>
+  </si>
+  <si>
+    <t>08:30 - 16:00</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Moises</t>
+  </si>
+  <si>
     <t>09:00 - 16:00</t>
   </si>
   <si>
-    <t>Agustin</t>
-  </si>
-  <si>
-    <t>16:30 - 23:30</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>13:00 - 20:00</t>
-  </si>
-  <si>
-    <t>Franco</t>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>15:00 - 22:00</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>16:00 - 22:00</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>08:30 - 17:00</t>
+  </si>
+  <si>
+    <t>12:00 - 21:00</t>
+  </si>
+  <si>
+    <t>Arantxa</t>
+  </si>
+  <si>
+    <t>11:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>09:00 - 18:00</t>
+  </si>
+  <si>
+    <t>Matias</t>
+  </si>
+  <si>
+    <t>pepito pruebaa</t>
+  </si>
+  <si>
+    <t>13:00 - 19:00</t>
   </si>
   <si>
     <t>14:00 - 21:00</t>
   </si>
   <si>
-    <t>Michelle</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Moises</t>
-  </si>
-  <si>
-    <t>14:30 - 20:30</t>
-  </si>
-  <si>
-    <t>08:30 - 16:00</t>
-  </si>
-  <si>
-    <t>Axel</t>
-  </si>
-  <si>
-    <t>Guillermo</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>08:30 - 17:00</t>
-  </si>
-  <si>
-    <t>17:30 - 23:30</t>
-  </si>
-  <si>
-    <t>13:00 - 19:00</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>16:00 - 22:00</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
-    <t>12:00 - 21:00</t>
-  </si>
-  <si>
-    <t>Arantxa</t>
-  </si>
-  <si>
-    <t>13:00 - 22:00</t>
-  </si>
-  <si>
-    <t>11:00 - 20:00</t>
-  </si>
-  <si>
-    <t>Carla</t>
-  </si>
-  <si>
-    <t>09:00 - 18:00</t>
-  </si>
-  <si>
-    <t>Matias</t>
-  </si>
-  <si>
-    <t>11:00 - 18:00</t>
-  </si>
-  <si>
-    <t>15:00 - 22:00</t>
-  </si>
-  <si>
-    <t>13:00 - 21:00</t>
-  </si>
-  <si>
-    <t>12:00 - 22:00</t>
-  </si>
-  <si>
-    <t>14:00 - 20:00</t>
-  </si>
-  <si>
-    <t>15:00 - 21:00</t>
-  </si>
-  <si>
     <t>09:00 - 18:30</t>
   </si>
   <si>
-    <t>10:00 - 19:00</t>
-  </si>
-  <si>
-    <t>08:30 - 17:30</t>
+    <t>11:00 - 19:30</t>
   </si>
 </sst>
 </file>
@@ -541,7 +529,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -580,9 +568,7 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
+      <c r="C2"/>
       <c r="D2" t="s">
         <v>10</v>
       </c>
@@ -590,9 +576,11 @@
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2"/>
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
       <c r="H2"/>
     </row>
     <row r="3" spans="1:8">
@@ -603,18 +591,18 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3"/>
       <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="G3"/>
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8">
@@ -636,30 +624,26 @@
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B5"/>
+      <c r="C5"/>
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E5"/>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
@@ -669,45 +653,45 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D6"/>
       <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6"/>
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B7"/>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7"/>
+        <v>23</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
       <c r="G7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -719,122 +703,122 @@
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8"/>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E9"/>
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G9"/>
+      <c r="G9" t="s">
+        <v>19</v>
+      </c>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10"/>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H10"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11"/>
+        <v>31</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="G11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H11"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
         <v>30</v>
       </c>
-      <c r="B12"/>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12"/>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
-      <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" t="s">
-        <v>15</v>
-      </c>
+      <c r="G12"/>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13"/>
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
       <c r="C13" t="s">
         <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F13"/>
       <c r="G13"/>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -849,7 +833,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -865,24 +849,22 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
+      <c r="G16"/>
       <c r="H16" t="s">
         <v>41</v>
       </c>
@@ -907,20 +889,18 @@
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
+      <c r="B18"/>
       <c r="C18"/>
       <c r="D18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" t="s">
-        <v>45</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E18"/>
       <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18"/>
+        <v>30</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
       <c r="H18" t="s">
         <v>19</v>
       </c>
@@ -943,6 +923,28 @@
       <c r="G19"/>
       <c r="H19" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -952,7 +954,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -998,7 +1000,7 @@
         <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
         <v>9</v>
@@ -1010,16 +1012,16 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
+      <c r="B3"/>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3"/>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
@@ -1033,10 +1035,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -1057,66 +1059,64 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5"/>
+      <c r="C5"/>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
+      <c r="B6"/>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6"/>
       <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6"/>
+        <v>16</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7"/>
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="H7" t="s">
-        <v>28</v>
-      </c>
+      <c r="H7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1125,123 +1125,119 @@
         <v>19</v>
       </c>
       <c r="D8"/>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
+      <c r="E8"/>
+      <c r="F8"/>
       <c r="G8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8"/>
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9"/>
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9"/>
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>14</v>
       </c>
       <c r="C10"/>
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
-        <v>15</v>
-      </c>
+      <c r="E10"/>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11"/>
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11"/>
-      <c r="H11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C12"/>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
+      <c r="D12"/>
       <c r="E12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12"/>
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13"/>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13"/>
       <c r="F13" t="s">
         <v>19</v>
       </c>
-      <c r="G13"/>
+      <c r="G13" t="s">
+        <v>19</v>
+      </c>
       <c r="H13" t="s">
         <v>19</v>
       </c>
@@ -1258,7 +1254,7 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1274,26 +1270,24 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
+      <c r="G16"/>
       <c r="H16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1309,7 +1303,7 @@
         <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -1317,22 +1311,22 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18"/>
-      <c r="D18" t="s">
-        <v>17</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18"/>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="H18"/>
+        <v>30</v>
+      </c>
+      <c r="G18"/>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
@@ -1353,6 +1347,28 @@
       <c r="H19" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1361,7 +1377,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1398,22 +1414,22 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2"/>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
+      <c r="H2"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
@@ -1424,37 +1440,37 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3"/>
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3" t="s">
-        <v>48</v>
-      </c>
+      <c r="H3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
@@ -1466,75 +1482,73 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
+      <c r="C5"/>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6"/>
-      <c r="C6"/>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
       <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="E6" t="s">
-        <v>45</v>
-      </c>
+      <c r="E6"/>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" t="s">
-        <v>21</v>
-      </c>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>47</v>
-      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7"/>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7"/>
+        <v>32</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
+      <c r="C8"/>
       <c r="D8"/>
       <c r="E8" t="s">
         <v>19</v>
@@ -1542,71 +1556,69 @@
       <c r="F8" t="s">
         <v>19</v>
       </c>
-      <c r="G8"/>
-      <c r="H8" t="s">
-        <v>15</v>
-      </c>
+      <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B9"/>
       <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" t="s">
         <v>14</v>
-      </c>
-      <c r="D9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" t="s">
-        <v>16</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
+      <c r="C10"/>
       <c r="D10" t="s">
         <v>19</v>
       </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
+      <c r="E10"/>
       <c r="F10"/>
       <c r="G10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10"/>
+        <v>38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11"/>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
         <v>19</v>
@@ -1615,45 +1627,43 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12" t="s">
         <v>30</v>
       </c>
-      <c r="B12"/>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>49</v>
-      </c>
       <c r="F12" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12"/>
+        <v>17</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13"/>
+      <c r="C13" t="s">
+        <v>30</v>
+      </c>
       <c r="D13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
       <c r="G13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="H13"/>
     </row>
@@ -1662,14 +1672,14 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1685,26 +1695,24 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H15" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
+      <c r="G16"/>
       <c r="H16" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1717,41 +1725,39 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
+      <c r="B18"/>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F18"/>
-      <c r="G18"/>
-      <c r="H18" t="s">
-        <v>19</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
+      <c r="B19"/>
       <c r="C19" t="s">
         <v>36</v>
       </c>
@@ -1763,7 +1769,29 @@
       </c>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19"/>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20"/>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1772,7 +1800,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1853,21 +1881,21 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4"/>
+      <c r="E4"/>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
       <c r="G4"/>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -1877,191 +1905,183 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6"/>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
+      <c r="C6"/>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6"/>
-      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
         <v>16</v>
       </c>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7"/>
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>49</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E7"/>
       <c r="F7"/>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
+      <c r="G7"/>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
       <c r="D8"/>
       <c r="E8" t="s">
         <v>19</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
+      <c r="F8"/>
       <c r="G8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H8"/>
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9"/>
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
       <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9"/>
       <c r="F9" t="s">
         <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9"/>
+        <v>19</v>
+      </c>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10"/>
+        <v>29</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="G10"/>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B11"/>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11"/>
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>23</v>
+      </c>
       <c r="F11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G11"/>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12"/>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C13" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E13"/>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
@@ -2073,14 +2093,14 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -2096,24 +2116,22 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" t="s">
-        <v>40</v>
-      </c>
+      <c r="G16"/>
       <c r="H16" t="s">
         <v>41</v>
       </c>
@@ -2128,31 +2146,31 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H17" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18"/>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18"/>
       <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="s">
-        <v>14</v>
-      </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H18"/>
     </row>
@@ -2160,21 +2178,43 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>36</v>
-      </c>
+      <c r="B19"/>
       <c r="C19" t="s">
         <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>36</v>
       </c>
-      <c r="E19"/>
+      <c r="E19" t="s">
+        <v>36</v>
+      </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limpieza de referencias de creado_por y arreglo error al crear notebook desde pagina haciendo que los ids sean consecutivos
</commit_message>
<xml_diff>
--- a/Backend/python/Carta_output.xlsx
+++ b/Backend/python/Carta_output.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>Trabajador</t>
   </si>
@@ -57,127 +57,148 @@
     <t>Jocelyn</t>
   </si>
   <si>
+    <t>11:00 - 21:00</t>
+  </si>
+  <si>
+    <t>09:00 - 19:00</t>
+  </si>
+  <si>
+    <t>Ignacio</t>
+  </si>
+  <si>
     <t>08:30 - 18:30</t>
   </si>
   <si>
     <t>08:00 - 18:00</t>
   </si>
   <si>
-    <t>11:00 - 21:00</t>
-  </si>
-  <si>
-    <t>Ignacio</t>
-  </si>
-  <si>
     <t>Ingrid</t>
   </si>
   <si>
+    <t>10:00 - 17:00</t>
+  </si>
+  <si>
+    <t>14:30 - 21:30</t>
+  </si>
+  <si>
+    <t>09:00 - 16:00</t>
+  </si>
+  <si>
+    <t>Agustin</t>
+  </si>
+  <si>
+    <t>16:30 - 23:30</t>
+  </si>
+  <si>
+    <t>Brian</t>
+  </si>
+  <si>
+    <t>12:00 - 19:00</t>
+  </si>
+  <si>
     <t>13:00 - 20:00</t>
   </si>
   <si>
-    <t>11:00 - 18:00</t>
-  </si>
-  <si>
-    <t>12:00 - 19:00</t>
-  </si>
-  <si>
-    <t>14:30 - 21:30</t>
-  </si>
-  <si>
-    <t>Agustin</t>
-  </si>
-  <si>
-    <t>16:30 - 23:30</t>
-  </si>
-  <si>
-    <t>Brian</t>
+    <t>Franco</t>
+  </si>
+  <si>
+    <t>08:30 - 16:00</t>
+  </si>
+  <si>
+    <t>Michelle</t>
+  </si>
+  <si>
+    <t>15:00 - 22:00</t>
+  </si>
+  <si>
+    <t>08:30 - 17:00</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Moises</t>
+  </si>
+  <si>
+    <t>Axel</t>
+  </si>
+  <si>
+    <t>12:00 - 18:30</t>
+  </si>
+  <si>
+    <t>Guillermo</t>
   </si>
   <si>
     <t>17:30 - 23:30</t>
   </si>
   <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>Manuel</t>
+  </si>
+  <si>
+    <t>12:00 - 21:00</t>
+  </si>
+  <si>
+    <t>10:00 - 19:00</t>
+  </si>
+  <si>
+    <t>Arantxa</t>
+  </si>
+  <si>
+    <t>13:00 - 22:00</t>
+  </si>
+  <si>
+    <t>12:00 - 20:30</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>11:00 - 20:00</t>
+  </si>
+  <si>
+    <t>Matias</t>
+  </si>
+  <si>
+    <t>13:00 - 19:00</t>
+  </si>
+  <si>
+    <t>16:00 - 22:00</t>
+  </si>
+  <si>
+    <t>asda</t>
+  </si>
+  <si>
+    <t>12:00 - 22:00</t>
+  </si>
+  <si>
+    <t>10:00 - 20:00</t>
+  </si>
+  <si>
+    <t>14:00 - 21:00</t>
+  </si>
+  <si>
     <t>13:00 - 21:00</t>
   </si>
   <si>
-    <t>10:00 - 17:00</t>
-  </si>
-  <si>
-    <t>Franco</t>
+    <t>09:00 - 18:00</t>
+  </si>
+  <si>
+    <t>11:00 - 17:00</t>
   </si>
   <si>
     <t>14:30 - 20:30</t>
   </si>
   <si>
-    <t>08:30 - 16:00</t>
-  </si>
-  <si>
-    <t>Michelle</t>
-  </si>
-  <si>
-    <t>Sebastian</t>
-  </si>
-  <si>
-    <t>Moises</t>
-  </si>
-  <si>
-    <t>09:00 - 16:00</t>
-  </si>
-  <si>
-    <t>Axel</t>
-  </si>
-  <si>
-    <t>15:00 - 22:00</t>
-  </si>
-  <si>
-    <t>Guillermo</t>
-  </si>
-  <si>
-    <t>Maria</t>
-  </si>
-  <si>
-    <t>Victoria</t>
-  </si>
-  <si>
-    <t>16:00 - 22:00</t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
-    <t>08:30 - 17:00</t>
-  </si>
-  <si>
-    <t>12:00 - 21:00</t>
-  </si>
-  <si>
-    <t>Arantxa</t>
-  </si>
-  <si>
-    <t>11:00 - 20:00</t>
-  </si>
-  <si>
-    <t>Carla</t>
-  </si>
-  <si>
-    <t>09:00 - 18:00</t>
-  </si>
-  <si>
-    <t>Matias</t>
-  </si>
-  <si>
-    <t>pepito pruebaa</t>
-  </si>
-  <si>
-    <t>13:00 - 19:00</t>
-  </si>
-  <si>
-    <t>14:00 - 21:00</t>
-  </si>
-  <si>
-    <t>09:00 - 18:30</t>
-  </si>
-  <si>
-    <t>11:00 - 19:30</t>
+    <t>10:00 - 18:30</t>
+  </si>
+  <si>
+    <t>14:00 - 20:00</t>
   </si>
 </sst>
 </file>
@@ -570,13 +591,13 @@
       </c>
       <c r="C2"/>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -585,42 +606,42 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3"/>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3"/>
-      <c r="H3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" t="s">
         <v>15</v>
-      </c>
-      <c r="D4"/>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
       </c>
       <c r="G4"/>
       <c r="H4" t="s">
@@ -631,59 +652,61 @@
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5"/>
-      <c r="C5"/>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5"/>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="D6"/>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6"/>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="B7"/>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
+      <c r="D7"/>
       <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F7"/>
       <c r="G7" t="s">
         <v>19</v>
       </c>
@@ -691,112 +714,102 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8"/>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8"/>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9"/>
+        <v>22</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
       <c r="F9" t="s">
         <v>19</v>
       </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
+      <c r="G9"/>
       <c r="H9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="G10"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11"/>
+        <v>31</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12"/>
+      <c r="G12" t="s">
+        <v>16</v>
+      </c>
       <c r="H12"/>
     </row>
     <row r="13" spans="1:8">
@@ -804,36 +817,36 @@
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
       <c r="E13" t="s">
-        <v>21</v>
-      </c>
-      <c r="F13"/>
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
       <c r="G13"/>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
+      <c r="H13"/>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -841,7 +854,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -849,22 +862,24 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" t="s">
         <v>38</v>
-      </c>
-      <c r="H15" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" t="s">
         <v>41</v>
       </c>
@@ -879,10 +894,10 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -890,19 +905,19 @@
         <v>44</v>
       </c>
       <c r="B18"/>
-      <c r="C18"/>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
       <c r="D18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18"/>
-      <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18"/>
+      <c r="G18"/>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -911,41 +926,41 @@
       </c>
       <c r="B19"/>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D20"/>
       <c r="E20" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20" t="s">
-        <v>46</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -991,60 +1006,60 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F2"/>
       <c r="G2"/>
-      <c r="H2"/>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1059,64 +1074,62 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5"/>
-      <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5"/>
+      <c r="H5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6"/>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
+      <c r="C6"/>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6"/>
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
       <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C7"/>
       <c r="D7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7"/>
+        <v>19</v>
+      </c>
+      <c r="E7"/>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
       <c r="G7"/>
-      <c r="H7"/>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1125,116 +1138,112 @@
         <v>19</v>
       </c>
       <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>19</v>
+      </c>
       <c r="G8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H8"/>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
+      <c r="B9"/>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F9"/>
       <c r="G9"/>
-      <c r="H9"/>
+      <c r="H9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10"/>
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
       <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G10"/>
       <c r="H10"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
         <v>31</v>
       </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
       <c r="F11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" t="s">
-        <v>14</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G11"/>
+      <c r="H11"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="B12"/>
       <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12" t="s">
-        <v>19</v>
-      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12"/>
       <c r="F12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
         <v>19</v>
       </c>
-      <c r="H12" t="s">
-        <v>17</v>
-      </c>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13"/>
-      <c r="C13" t="s">
-        <v>16</v>
-      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13"/>
       <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13"/>
       <c r="G13" t="s">
         <v>19</v>
       </c>
@@ -1247,14 +1256,14 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1262,7 +1271,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1270,24 +1279,26 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1300,73 +1311,71 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
+      <c r="B18"/>
       <c r="C18" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D18"/>
       <c r="E18" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="G18"/>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" t="s">
-        <v>36</v>
-      </c>
+      <c r="H19"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20"/>
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" t="s">
-        <v>19</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E20"/>
       <c r="F20" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H20"/>
     </row>
@@ -1413,67 +1422,65 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2"/>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="G2"/>
-      <c r="H2"/>
+      <c r="H2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="B3"/>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H3"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
+      <c r="D4"/>
+      <c r="E4"/>
       <c r="F4" t="s">
         <v>16</v>
       </c>
       <c r="G4"/>
-      <c r="H4"/>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
@@ -1482,73 +1489,71 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5"/>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F5" t="s">
         <v>19</v>
       </c>
       <c r="G5"/>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
+      <c r="H5"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6"/>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>19</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6"/>
       <c r="H6"/>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="B7"/>
       <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7"/>
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
       <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7"/>
-      <c r="H7" t="s">
-        <v>46</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8"/>
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
       <c r="D8"/>
       <c r="E8" t="s">
         <v>19</v>
@@ -1557,7 +1562,7 @@
         <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="H8"/>
     </row>
@@ -1565,121 +1570,117 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9"/>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>16</v>
-      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
       <c r="E9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G9"/>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10"/>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10"/>
-      <c r="F10"/>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
       <c r="G10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H10"/>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D11" t="s">
-        <v>17</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
       <c r="E11"/>
-      <c r="F11" t="s">
-        <v>23</v>
-      </c>
+      <c r="F11"/>
       <c r="G11" t="s">
         <v>19</v>
       </c>
-      <c r="H11"/>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12"/>
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H12" t="s">
-        <v>23</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13"/>
+      <c r="C13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13"/>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13"/>
+        <v>16</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -1687,7 +1688,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -1695,24 +1696,26 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -1725,32 +1728,32 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18"/>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" t="s">
-        <v>19</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
@@ -1758,40 +1761,40 @@
         <v>18</v>
       </c>
       <c r="B19"/>
-      <c r="C19" t="s">
-        <v>36</v>
-      </c>
+      <c r="C19"/>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20"/>
-      <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20"/>
-      <c r="H20" t="s">
-        <v>26</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20"/>
+      <c r="F20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1836,84 +1839,78 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
+      <c r="B2"/>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2"/>
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
       <c r="H2"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3"/>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3"/>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="H3"/>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4"/>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4"/>
       <c r="G4"/>
-      <c r="H4" t="s">
-        <v>17</v>
-      </c>
+      <c r="H4"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
+      <c r="B5"/>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
+      <c r="E5"/>
       <c r="F5" t="s">
         <v>19</v>
       </c>
@@ -1924,47 +1921,51 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6"/>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
       <c r="C6"/>
       <c r="D6" t="s">
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6"/>
+        <v>19</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" t="s">
         <v>23</v>
       </c>
+      <c r="B7"/>
       <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7"/>
-      <c r="H7" t="s">
-        <v>26</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="D7"/>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8"/>
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8" t="s">
@@ -1972,10 +1973,10 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -1983,109 +1984,105 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D9"/>
-      <c r="E9"/>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
       <c r="F9" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" t="s">
-        <v>19</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="G9"/>
+      <c r="H9"/>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10"/>
-      <c r="C10" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10"/>
       <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10"/>
+        <v>16</v>
+      </c>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10" t="s">
+        <v>27</v>
+      </c>
       <c r="H10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11"/>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11"/>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11"/>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12"/>
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>30</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E12"/>
       <c r="F12" t="s">
         <v>19</v>
       </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12"/>
+      <c r="G12"/>
+      <c r="H12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13"/>
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>19</v>
+      </c>
       <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" t="s">
-        <v>19</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G13"/>
       <c r="H13"/>
     </row>
     <row r="14" spans="1:8">
@@ -2093,14 +2090,14 @@
         <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="H14" t="s">
         <v>19</v>
@@ -2108,7 +2105,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15"/>
       <c r="C15"/>
@@ -2116,24 +2113,26 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16"/>
+      <c r="G16" t="s">
+        <v>40</v>
+      </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -2146,75 +2145,73 @@
       <c r="E17"/>
       <c r="F17"/>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18"/>
+      <c r="B18"/>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" t="s">
-        <v>17</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="G18"/>
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19"/>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
       <c r="C19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
-      <c r="H19" t="s">
-        <v>36</v>
-      </c>
+      <c r="H19"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D20"/>
       <c r="E20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20"/>
-      <c r="G20" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20"/>
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20"/>
+      <c r="H20" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>